<commit_message>
fixed bug on dfa
</commit_message>
<xml_diff>
--- a/dfa simplified.xlsx
+++ b/dfa simplified.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1" xr2:uid="{97A9BE92-959E-40FC-957B-6C09EAEF31F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{97A9BE92-959E-40FC-957B-6C09EAEF31F7}"/>
   </bookViews>
   <sheets>
     <sheet name="new (2)" sheetId="12" r:id="rId1"/>
@@ -466,7 +466,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -764,12 +764,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64EC608-A832-4A52-9803-5E1D2044E9D9}">
   <dimension ref="A1:N93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49:D92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -931,7 +931,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G5" s="1">
         <v>14</v>
@@ -2354,7 +2354,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C2:K2)</f>
+        <f t="shared" ref="D49:D92" si="0">_xlfn.TEXTJOIN(",",,C2:K2)</f>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
         <v>2</v>
       </c>
       <c r="D50" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C3:K3)</f>
+        <f t="shared" si="0"/>
         <v>8,0,12,13,0,18,0,23,0</v>
       </c>
     </row>
@@ -2372,7 +2372,7 @@
         <v>3</v>
       </c>
       <c r="D51" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C4:K4)</f>
+        <f t="shared" si="0"/>
         <v>0,9,11,0,14,17,0,22,0</v>
       </c>
     </row>
@@ -2381,8 +2381,8 @@
         <v>4</v>
       </c>
       <c r="D52" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C5:K5)</f>
-        <v>8,9,10,2,14,15,0,21,0</v>
+        <f t="shared" si="0"/>
+        <v>8,9,10,13,14,15,0,21,0</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.25">
@@ -2390,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="D53" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C6:K6)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,20,0,0</v>
       </c>
     </row>
@@ -2399,7 +2399,7 @@
         <v>6</v>
       </c>
       <c r="D54" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C7:K7)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,19,0,0</v>
       </c>
     </row>
@@ -2408,7 +2408,7 @@
         <v>7</v>
       </c>
       <c r="D55" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C8:K8)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,16,0,0</v>
       </c>
     </row>
@@ -2417,7 +2417,7 @@
         <v>8</v>
       </c>
       <c r="D56" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C9:K9)</f>
+        <f t="shared" si="0"/>
         <v>24,0,28,29,0,34,0,39,0</v>
       </c>
     </row>
@@ -2426,7 +2426,7 @@
         <v>9</v>
       </c>
       <c r="D57" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C10:K10)</f>
+        <f t="shared" si="0"/>
         <v>0,25,27,0,30,33,0,38,0</v>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
         <v>10</v>
       </c>
       <c r="D58" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C11:K11)</f>
+        <f t="shared" si="0"/>
         <v>24,25,26,29,30,31,0,37,0</v>
       </c>
     </row>
@@ -2444,7 +2444,7 @@
         <v>11</v>
       </c>
       <c r="D59" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C12:K12)</f>
+        <f t="shared" si="0"/>
         <v>0,25,27,0,30,33,0,38,0</v>
       </c>
     </row>
@@ -2453,7 +2453,7 @@
         <v>12</v>
       </c>
       <c r="D60" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C13:K13)</f>
+        <f t="shared" si="0"/>
         <v>24,0,28,29,0,34,0,39,0</v>
       </c>
     </row>
@@ -2462,7 +2462,7 @@
         <v>13</v>
       </c>
       <c r="D61" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C14:K14)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,36,0,0</v>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
         <v>14</v>
       </c>
       <c r="D62" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C15:K15)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,35,0,0</v>
       </c>
     </row>
@@ -2480,7 +2480,7 @@
         <v>15</v>
       </c>
       <c r="D63" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C16:K16)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,32,0,0</v>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
         <v>59</v>
       </c>
       <c r="D64" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C17:K17)</f>
+        <f t="shared" si="0"/>
         <v>24,25,26,29,30,31,0,37,0</v>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
         <v>60</v>
       </c>
       <c r="D65" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C18:K18)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,35,0,0</v>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
         <v>61</v>
       </c>
       <c r="D66" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C19:K19)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,36,0,0</v>
       </c>
     </row>
@@ -2516,7 +2516,7 @@
         <v>62</v>
       </c>
       <c r="D67" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C20:K20)</f>
+        <f t="shared" si="0"/>
         <v>0,25,27,0,30,33,0,38,0</v>
       </c>
     </row>
@@ -2525,7 +2525,7 @@
         <v>63</v>
       </c>
       <c r="D68" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C21:K21)</f>
+        <f t="shared" si="0"/>
         <v>24,0,28,29,0,34,0,39,0</v>
       </c>
     </row>
@@ -2534,7 +2534,7 @@
         <v>64</v>
       </c>
       <c r="D69" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C22:K22)</f>
+        <f t="shared" si="0"/>
         <v>24,25,26,29,30,31,0,37,0</v>
       </c>
     </row>
@@ -2543,7 +2543,7 @@
         <v>65</v>
       </c>
       <c r="D70" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C23:K23)</f>
+        <f t="shared" si="0"/>
         <v>0,25,27,0,30,33,0,38,0</v>
       </c>
     </row>
@@ -2552,7 +2552,7 @@
         <v>66</v>
       </c>
       <c r="D71" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C24:K24)</f>
+        <f t="shared" si="0"/>
         <v>24,0,28,29,0,34,0,39,0</v>
       </c>
     </row>
@@ -2561,7 +2561,7 @@
         <v>67</v>
       </c>
       <c r="D72" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C25:K25)</f>
+        <f t="shared" si="0"/>
         <v>40,0,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
         <v>68</v>
       </c>
       <c r="D73" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C26:K26)</f>
+        <f t="shared" si="0"/>
         <v>0,41,0,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2579,7 +2579,7 @@
         <v>69</v>
       </c>
       <c r="D74" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C27:K27)</f>
+        <f t="shared" si="0"/>
         <v>40,41,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2588,7 +2588,7 @@
         <v>70</v>
       </c>
       <c r="D75" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C28:K28)</f>
+        <f t="shared" si="0"/>
         <v>0,41,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2597,7 +2597,7 @@
         <v>71</v>
       </c>
       <c r="D76" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C29:K29)</f>
+        <f t="shared" si="0"/>
         <v>40,0,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2606,7 +2606,7 @@
         <v>72</v>
       </c>
       <c r="D77" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C30:K30)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,43,0,0</v>
       </c>
     </row>
@@ -2615,7 +2615,7 @@
         <v>73</v>
       </c>
       <c r="D78" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C31:K31)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,43,0,0</v>
       </c>
     </row>
@@ -2624,7 +2624,7 @@
         <v>74</v>
       </c>
       <c r="D79" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C32:K32)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,43,0,0</v>
       </c>
     </row>
@@ -2633,7 +2633,7 @@
         <v>75</v>
       </c>
       <c r="D80" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C33:K33)</f>
+        <f t="shared" si="0"/>
         <v>40,41,42,0,0,0,44,0,0</v>
       </c>
     </row>
@@ -2642,7 +2642,7 @@
         <v>76</v>
       </c>
       <c r="D81" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C34:K34)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,43,0,0</v>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
         <v>77</v>
       </c>
       <c r="D82" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C35:K35)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,43,0,0</v>
       </c>
     </row>
@@ -2660,7 +2660,7 @@
         <v>78</v>
       </c>
       <c r="D83" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C36:K36)</f>
+        <f t="shared" si="0"/>
         <v>0,41,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2669,7 +2669,7 @@
         <v>79</v>
       </c>
       <c r="D84" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C37:K37)</f>
+        <f t="shared" si="0"/>
         <v>40,0,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2678,7 +2678,7 @@
         <v>80</v>
       </c>
       <c r="D85" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C38:K38)</f>
+        <f t="shared" si="0"/>
         <v>40,41,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2687,7 +2687,7 @@
         <v>81</v>
       </c>
       <c r="D86" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C39:K39)</f>
+        <f t="shared" si="0"/>
         <v>0,41,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2696,7 +2696,7 @@
         <v>86</v>
       </c>
       <c r="D87" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C40:K40)</f>
+        <f t="shared" si="0"/>
         <v>40,0,42,0,0,0,0,44,0</v>
       </c>
     </row>
@@ -2705,7 +2705,7 @@
         <v>87</v>
       </c>
       <c r="D88" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C41:K41)</f>
+        <f t="shared" si="0"/>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2714,7 +2714,7 @@
         <v>88</v>
       </c>
       <c r="D89" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C42:K42)</f>
+        <f t="shared" si="0"/>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
         <v>89</v>
       </c>
       <c r="D90" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C43:K43)</f>
+        <f t="shared" si="0"/>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2732,7 +2732,7 @@
         <v>90</v>
       </c>
       <c r="D91" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C44:K44)</f>
+        <f t="shared" si="0"/>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
         <v>91</v>
       </c>
       <c r="D92" t="str">
-        <f>_xlfn.TEXTJOIN(",",,C45:K45)</f>
+        <f t="shared" si="0"/>
         <v>2,3,4,5,6,7,0,0,1</v>
       </c>
     </row>
@@ -2788,11 +2788,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07F4D98-D97B-4BD8-A169-0D709CD97346}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>